<commit_message>
updates in week 6
</commit_message>
<xml_diff>
--- a/BusinessDocuments/_Project Delivery Schedule_Spring 2020.xlsx
+++ b/BusinessDocuments/_Project Delivery Schedule_Spring 2020.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Yuri Folder\MY Doc\MyPapers\My Training Classes\Pace Courses\Pace CS691\2020 Spring\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sunco\Google Drive (scottsun17@gmail.com)\Computer Science Project\BundleBid\BusinessDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C01B687-3CCF-4B43-B877-EBD8D5661D5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE47DCC2-07EC-4608-BD50-818E6F8B135C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Schedule" sheetId="16" r:id="rId1"/>
@@ -1471,6 +1471,24 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1488,24 +1506,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1888,45 +1888,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D68D90BE-A99B-4831-BB7D-713F3AE5C123}">
   <dimension ref="A1:S27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="43.5703125" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="43.5546875" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" customWidth="1"/>
     <col min="4" max="4" width="28" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" style="37" customWidth="1"/>
-    <col min="6" max="12" width="9.140625" style="37"/>
-    <col min="13" max="13" width="9.7109375" style="37" customWidth="1"/>
-    <col min="14" max="19" width="9.140625" style="37"/>
+    <col min="5" max="5" width="11.109375" style="37" customWidth="1"/>
+    <col min="6" max="12" width="9.109375" style="37"/>
+    <col min="13" max="13" width="9.6640625" style="37" customWidth="1"/>
+    <col min="14" max="19" width="9.109375" style="37"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="14"/>
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
       <c r="D1" s="14"/>
-      <c r="E1" s="124" t="s">
+      <c r="E1" s="118" t="s">
         <v>147</v>
       </c>
-      <c r="F1" s="124"/>
-      <c r="G1" s="124"/>
-      <c r="H1" s="124"/>
-      <c r="I1" s="124"/>
-      <c r="J1" s="124"/>
-      <c r="K1" s="124"/>
-      <c r="L1" s="124"/>
-      <c r="M1" s="124"/>
-      <c r="N1" s="124"/>
-      <c r="O1" s="124"/>
-      <c r="P1" s="124"/>
-      <c r="Q1" s="124"/>
-      <c r="R1" s="124"/>
-      <c r="S1" s="124"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F1" s="118"/>
+      <c r="G1" s="118"/>
+      <c r="H1" s="118"/>
+      <c r="I1" s="118"/>
+      <c r="J1" s="118"/>
+      <c r="K1" s="118"/>
+      <c r="L1" s="118"/>
+      <c r="M1" s="118"/>
+      <c r="N1" s="118"/>
+      <c r="O1" s="118"/>
+      <c r="P1" s="118"/>
+      <c r="Q1" s="118"/>
+      <c r="R1" s="118"/>
+      <c r="S1" s="118"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
@@ -1947,7 +1947,7 @@
       <c r="R2" s="15"/>
       <c r="S2" s="15"/>
     </row>
-    <row r="3" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
         <v>29</v>
       </c>
@@ -2006,7 +2006,7 @@
         <v>43956</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="20">
         <v>1</v>
       </c>
@@ -2026,7 +2026,7 @@
       <c r="I4" s="80"/>
       <c r="J4" s="80"/>
       <c r="K4" s="80"/>
-      <c r="L4" s="125" t="s">
+      <c r="L4" s="119" t="s">
         <v>148</v>
       </c>
       <c r="M4" s="82"/>
@@ -2037,7 +2037,7 @@
       <c r="R4" s="80"/>
       <c r="S4" s="82"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="20">
         <v>2</v>
       </c>
@@ -2057,7 +2057,7 @@
       <c r="I5" s="15"/>
       <c r="J5" s="15"/>
       <c r="K5" s="15"/>
-      <c r="L5" s="126"/>
+      <c r="L5" s="120"/>
       <c r="M5" s="85"/>
       <c r="N5" s="15"/>
       <c r="O5" s="15"/>
@@ -2066,8 +2066,8 @@
       <c r="R5" s="15"/>
       <c r="S5" s="85"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="115">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A6" s="121">
         <v>3</v>
       </c>
       <c r="B6" s="21" t="s">
@@ -2076,7 +2076,7 @@
       <c r="C6" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="119" t="s">
+      <c r="D6" s="125" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="72"/>
@@ -2086,7 +2086,7 @@
       <c r="I6" s="15"/>
       <c r="J6" s="15"/>
       <c r="K6" s="15"/>
-      <c r="L6" s="126"/>
+      <c r="L6" s="120"/>
       <c r="M6" s="85"/>
       <c r="N6" s="15"/>
       <c r="O6" s="15"/>
@@ -2095,15 +2095,15 @@
       <c r="R6" s="15"/>
       <c r="S6" s="85"/>
     </row>
-    <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="116"/>
+    <row r="7" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="122"/>
       <c r="B7" s="21" t="s">
         <v>35</v>
       </c>
       <c r="C7" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="120"/>
+      <c r="D7" s="126"/>
       <c r="E7" s="72"/>
       <c r="F7" s="15"/>
       <c r="G7" s="104"/>
@@ -2111,7 +2111,7 @@
       <c r="I7" s="106"/>
       <c r="J7" s="15"/>
       <c r="K7" s="15"/>
-      <c r="L7" s="126"/>
+      <c r="L7" s="120"/>
       <c r="M7" s="85"/>
       <c r="N7" s="15"/>
       <c r="O7" s="15"/>
@@ -2120,7 +2120,7 @@
       <c r="R7" s="15"/>
       <c r="S7" s="85"/>
     </row>
-    <row r="8" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="20">
         <v>4</v>
       </c>
@@ -2140,7 +2140,7 @@
       <c r="I8" s="106"/>
       <c r="J8" s="15"/>
       <c r="K8" s="15"/>
-      <c r="L8" s="126"/>
+      <c r="L8" s="120"/>
       <c r="M8" s="85"/>
       <c r="N8" s="15"/>
       <c r="O8" s="15"/>
@@ -2149,11 +2149,11 @@
       <c r="R8" s="15"/>
       <c r="S8" s="85"/>
     </row>
-    <row r="9" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="115">
+    <row r="9" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="121">
         <v>5</v>
       </c>
-      <c r="B9" s="119" t="s">
+      <c r="B9" s="125" t="s">
         <v>37</v>
       </c>
       <c r="C9" s="97" t="s">
@@ -2169,7 +2169,7 @@
       <c r="I9" s="45"/>
       <c r="J9" s="15"/>
       <c r="K9" s="15"/>
-      <c r="L9" s="126"/>
+      <c r="L9" s="120"/>
       <c r="M9" s="107"/>
       <c r="N9" s="15"/>
       <c r="O9" s="15"/>
@@ -2178,9 +2178,9 @@
       <c r="R9" s="15"/>
       <c r="S9" s="85"/>
     </row>
-    <row r="10" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="116"/>
-      <c r="B10" s="120"/>
+    <row r="10" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="122"/>
+      <c r="B10" s="126"/>
       <c r="C10" s="98" t="s">
         <v>17</v>
       </c>
@@ -2194,7 +2194,7 @@
       <c r="I10" s="45"/>
       <c r="J10" s="15"/>
       <c r="K10" s="15"/>
-      <c r="L10" s="126"/>
+      <c r="L10" s="120"/>
       <c r="M10" s="107"/>
       <c r="N10" s="15"/>
       <c r="O10" s="15"/>
@@ -2203,11 +2203,11 @@
       <c r="R10" s="15"/>
       <c r="S10" s="85"/>
     </row>
-    <row r="11" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="115">
+    <row r="11" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="121">
         <v>6</v>
       </c>
-      <c r="B11" s="119" t="s">
+      <c r="B11" s="125" t="s">
         <v>72</v>
       </c>
       <c r="C11" s="97" t="s">
@@ -2223,7 +2223,7 @@
       <c r="I11" s="15"/>
       <c r="J11" s="103"/>
       <c r="K11" s="108"/>
-      <c r="L11" s="126"/>
+      <c r="L11" s="120"/>
       <c r="M11" s="85"/>
       <c r="N11" s="106"/>
       <c r="O11" s="15"/>
@@ -2232,9 +2232,9 @@
       <c r="R11" s="15"/>
       <c r="S11" s="85"/>
     </row>
-    <row r="12" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="116"/>
-      <c r="B12" s="120"/>
+    <row r="12" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="122"/>
+      <c r="B12" s="126"/>
       <c r="C12" s="98" t="s">
         <v>17</v>
       </c>
@@ -2248,7 +2248,7 @@
       <c r="I12" s="15"/>
       <c r="J12" s="103"/>
       <c r="K12" s="108"/>
-      <c r="L12" s="126"/>
+      <c r="L12" s="120"/>
       <c r="M12" s="107"/>
       <c r="N12" s="27"/>
       <c r="O12" s="15"/>
@@ -2257,11 +2257,11 @@
       <c r="R12" s="15"/>
       <c r="S12" s="85"/>
     </row>
-    <row r="13" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="115">
+    <row r="13" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="121">
         <v>7</v>
       </c>
-      <c r="B13" s="117" t="s">
+      <c r="B13" s="123" t="s">
         <v>73</v>
       </c>
       <c r="C13" s="73" t="s">
@@ -2277,7 +2277,7 @@
       <c r="I13" s="15"/>
       <c r="J13" s="15"/>
       <c r="K13" s="103"/>
-      <c r="L13" s="126"/>
+      <c r="L13" s="120"/>
       <c r="M13" s="107"/>
       <c r="N13" s="15"/>
       <c r="O13" s="15"/>
@@ -2286,9 +2286,9 @@
       <c r="R13" s="15"/>
       <c r="S13" s="85"/>
     </row>
-    <row r="14" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="116"/>
-      <c r="B14" s="118"/>
+    <row r="14" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="122"/>
+      <c r="B14" s="124"/>
       <c r="C14" s="74" t="s">
         <v>130</v>
       </c>
@@ -2304,7 +2304,7 @@
       <c r="K14" s="109" t="s">
         <v>43</v>
       </c>
-      <c r="L14" s="126"/>
+      <c r="L14" s="120"/>
       <c r="M14" s="107"/>
       <c r="N14" s="15"/>
       <c r="O14" s="15"/>
@@ -2313,7 +2313,7 @@
       <c r="R14" s="15"/>
       <c r="S14" s="85"/>
     </row>
-    <row r="15" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="25">
         <v>8</v>
       </c>
@@ -2333,7 +2333,7 @@
       <c r="I15" s="15"/>
       <c r="J15" s="15"/>
       <c r="K15" s="15"/>
-      <c r="L15" s="126"/>
+      <c r="L15" s="120"/>
       <c r="M15" s="110" t="s">
         <v>45</v>
       </c>
@@ -2344,7 +2344,7 @@
       <c r="R15" s="15"/>
       <c r="S15" s="85"/>
     </row>
-    <row r="16" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="20">
         <v>9</v>
       </c>
@@ -2364,7 +2364,7 @@
       <c r="I16" s="15"/>
       <c r="J16" s="15"/>
       <c r="K16" s="15"/>
-      <c r="L16" s="126"/>
+      <c r="L16" s="120"/>
       <c r="M16" s="85"/>
       <c r="N16" s="45"/>
       <c r="O16" s="27"/>
@@ -2373,7 +2373,7 @@
       <c r="R16" s="15"/>
       <c r="S16" s="85"/>
     </row>
-    <row r="17" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="20">
         <v>10</v>
       </c>
@@ -2393,7 +2393,7 @@
       <c r="I17" s="15"/>
       <c r="J17" s="15"/>
       <c r="K17" s="15"/>
-      <c r="L17" s="126"/>
+      <c r="L17" s="120"/>
       <c r="M17" s="85"/>
       <c r="N17" s="27"/>
       <c r="O17" s="45"/>
@@ -2402,7 +2402,7 @@
       <c r="R17" s="15"/>
       <c r="S17" s="85"/>
     </row>
-    <row r="18" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="20">
         <v>11</v>
       </c>
@@ -2422,7 +2422,7 @@
       <c r="I18" s="15"/>
       <c r="J18" s="15"/>
       <c r="K18" s="15"/>
-      <c r="L18" s="126"/>
+      <c r="L18" s="120"/>
       <c r="M18" s="85"/>
       <c r="N18" s="15"/>
       <c r="O18" s="28"/>
@@ -2431,8 +2431,8 @@
       <c r="R18" s="15"/>
       <c r="S18" s="87"/>
     </row>
-    <row r="19" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="115">
+    <row r="19" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="121">
         <v>12</v>
       </c>
       <c r="B19" s="21" t="s">
@@ -2451,7 +2451,7 @@
       <c r="I19" s="15"/>
       <c r="J19" s="15"/>
       <c r="K19" s="15"/>
-      <c r="L19" s="126"/>
+      <c r="L19" s="120"/>
       <c r="M19" s="85"/>
       <c r="N19" s="15"/>
       <c r="O19" s="15"/>
@@ -2460,8 +2460,8 @@
       <c r="R19" s="27"/>
       <c r="S19" s="87"/>
     </row>
-    <row r="20" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="116"/>
+    <row r="20" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="122"/>
       <c r="B20" s="29" t="s">
         <v>77</v>
       </c>
@@ -2478,7 +2478,7 @@
       <c r="I20" s="15"/>
       <c r="J20" s="15"/>
       <c r="K20" s="15"/>
-      <c r="L20" s="126"/>
+      <c r="L20" s="120"/>
       <c r="M20" s="85"/>
       <c r="N20" s="15"/>
       <c r="O20" s="15"/>
@@ -2489,7 +2489,7 @@
       <c r="R20" s="27"/>
       <c r="S20" s="87"/>
     </row>
-    <row r="21" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="30">
         <v>13</v>
       </c>
@@ -2509,7 +2509,7 @@
       <c r="I21" s="15"/>
       <c r="J21" s="15"/>
       <c r="K21" s="15"/>
-      <c r="L21" s="126"/>
+      <c r="L21" s="120"/>
       <c r="M21" s="85"/>
       <c r="N21" s="15"/>
       <c r="O21" s="15"/>
@@ -2520,7 +2520,7 @@
       </c>
       <c r="S21" s="87"/>
     </row>
-    <row r="22" spans="1:19" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="33">
         <v>14</v>
       </c>
@@ -2540,7 +2540,7 @@
       <c r="I22" s="15"/>
       <c r="J22" s="15"/>
       <c r="K22" s="15"/>
-      <c r="L22" s="126"/>
+      <c r="L22" s="120"/>
       <c r="M22" s="85"/>
       <c r="N22" s="15"/>
       <c r="O22" s="15"/>
@@ -2551,38 +2551,38 @@
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A23" s="14"/>
       <c r="B23" s="14"/>
       <c r="C23" s="14"/>
       <c r="D23" s="113" t="s">
         <v>59</v>
       </c>
-      <c r="E23" s="121" t="s">
+      <c r="E23" s="115" t="s">
         <v>4</v>
       </c>
-      <c r="F23" s="122"/>
-      <c r="G23" s="122"/>
-      <c r="H23" s="123" t="s">
+      <c r="F23" s="116"/>
+      <c r="G23" s="116"/>
+      <c r="H23" s="117" t="s">
         <v>80</v>
       </c>
-      <c r="I23" s="123"/>
-      <c r="J23" s="123"/>
-      <c r="K23" s="123"/>
-      <c r="L23" s="123"/>
-      <c r="M23" s="123"/>
-      <c r="N23" s="122" t="s">
+      <c r="I23" s="117"/>
+      <c r="J23" s="117"/>
+      <c r="K23" s="117"/>
+      <c r="L23" s="117"/>
+      <c r="M23" s="117"/>
+      <c r="N23" s="116" t="s">
         <v>149</v>
       </c>
-      <c r="O23" s="122"/>
-      <c r="P23" s="122"/>
-      <c r="Q23" s="123" t="s">
+      <c r="O23" s="116"/>
+      <c r="P23" s="116"/>
+      <c r="Q23" s="117" t="s">
         <v>14</v>
       </c>
-      <c r="R23" s="123"/>
-      <c r="S23" s="123"/>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R23" s="117"/>
+      <c r="S23" s="117"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="14"/>
       <c r="B24" s="14"/>
       <c r="C24" s="14"/>
@@ -2603,17 +2603,11 @@
       <c r="R24" s="15"/>
       <c r="S24" s="15"/>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="E27" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="H23:M23"/>
-    <mergeCell ref="N23:P23"/>
-    <mergeCell ref="Q23:S23"/>
-    <mergeCell ref="E1:S1"/>
-    <mergeCell ref="L4:L22"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="A19:A20"/>
@@ -2623,6 +2617,12 @@
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="B11:B12"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="H23:M23"/>
+    <mergeCell ref="N23:P23"/>
+    <mergeCell ref="Q23:S23"/>
+    <mergeCell ref="E1:S1"/>
+    <mergeCell ref="L4:L22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2636,27 +2636,27 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="1" max="1" width="23.5546875" customWidth="1"/>
     <col min="2" max="2" width="7" customWidth="1"/>
     <col min="3" max="3" width="49" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="124" t="s">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="118" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="124"/>
-      <c r="C1" s="124"/>
-      <c r="D1" s="124"/>
-      <c r="E1" s="124"/>
-      <c r="F1" s="124"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+      <c r="F1" s="118"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
@@ -2664,7 +2664,7 @@
       <c r="E2" s="14"/>
       <c r="F2" s="41"/>
     </row>
-    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -2684,7 +2684,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
@@ -2704,7 +2704,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="12">
         <v>2</v>
@@ -2722,7 +2722,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
@@ -2742,7 +2742,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="12">
         <v>4</v>
@@ -2760,7 +2760,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="12">
         <v>5</v>
@@ -2778,7 +2778,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="12">
         <v>6</v>
@@ -2796,7 +2796,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="12">
         <v>7</v>
@@ -2814,7 +2814,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="12">
         <v>8</v>
@@ -2832,7 +2832,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="12">
         <v>9</v>
@@ -2850,7 +2850,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="12">
         <v>10</v>
@@ -2868,7 +2868,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="12">
         <v>11</v>
@@ -2886,7 +2886,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>12</v>
       </c>
@@ -2906,7 +2906,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="12">
         <v>13</v>
@@ -2924,7 +2924,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="12">
         <v>14</v>
@@ -2942,7 +2942,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="12">
         <v>15</v>
@@ -2960,7 +2960,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>13</v>
       </c>
@@ -2980,7 +2980,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="6" t="s">
         <v>14</v>
       </c>
@@ -3000,7 +3000,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
         <v>21</v>
       </c>
@@ -3020,7 +3020,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A22" s="14"/>
       <c r="B22" s="14"/>
       <c r="C22" s="14"/>
@@ -3046,20 +3046,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" customWidth="1"/>
     <col min="2" max="2" width="7" style="1" customWidth="1"/>
-    <col min="3" max="3" width="31.42578125" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" customWidth="1"/>
-    <col min="5" max="5" width="71.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="31.44140625" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" customWidth="1"/>
+    <col min="5" max="5" width="71.5546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="127" t="s">
         <v>89</v>
       </c>
@@ -3068,7 +3068,7 @@
       <c r="D1" s="127"/>
       <c r="E1" s="127"/>
     </row>
-    <row r="2" spans="1:5" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="128" t="s">
         <v>93</v>
       </c>
@@ -3077,7 +3077,7 @@
       <c r="D2" s="129"/>
       <c r="E2" s="130"/>
     </row>
-    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -3094,7 +3094,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A4" s="133" t="s">
         <v>4</v>
       </c>
@@ -3111,7 +3111,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="134"/>
       <c r="B5" s="48">
         <v>2</v>
@@ -3126,7 +3126,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="185.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="185.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="133" t="s">
         <v>8</v>
       </c>
@@ -3143,7 +3143,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="201" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="201" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="135"/>
       <c r="B7" s="48">
         <v>4</v>
@@ -3158,7 +3158,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="99.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="135"/>
       <c r="B8" s="48">
         <v>5</v>
@@ -3173,7 +3173,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="219.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="219.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="135"/>
       <c r="B9" s="48">
         <v>6</v>
@@ -3188,7 +3188,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="128.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="128.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="135"/>
       <c r="B10" s="48" t="s">
         <v>33</v>
@@ -3203,7 +3203,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="251.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="251.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="135"/>
       <c r="B11" s="48">
         <v>7</v>
@@ -3218,7 +3218,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="144" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="144" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="135"/>
       <c r="B12" s="48">
         <v>8</v>
@@ -3233,7 +3233,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="135"/>
       <c r="B13" s="51">
         <v>9</v>
@@ -3248,7 +3248,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="146.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="146.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="135"/>
       <c r="B14" s="51">
         <v>10</v>
@@ -3263,7 +3263,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="84.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="135"/>
       <c r="B15" s="48">
         <v>10</v>
@@ -3278,7 +3278,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="114" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="114" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="134"/>
       <c r="B16" s="48">
         <v>11</v>
@@ -3293,7 +3293,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="133" t="s">
         <v>12</v>
       </c>
@@ -3310,7 +3310,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="135"/>
       <c r="B18" s="48">
         <v>13</v>
@@ -3323,7 +3323,7 @@
       </c>
       <c r="E18" s="132"/>
     </row>
-    <row r="19" spans="1:5" ht="174" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="174" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="135"/>
       <c r="B19" s="48">
         <v>14</v>
@@ -3338,7 +3338,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="97.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="134"/>
       <c r="B20" s="48">
         <v>15</v>
@@ -3353,7 +3353,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="94" t="s">
         <v>13</v>
       </c>
@@ -3370,7 +3370,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="171" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="171" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="69" t="s">
         <v>14</v>
       </c>
@@ -3387,7 +3387,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="138.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="138.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="70" t="s">
         <v>21</v>
       </c>
@@ -3404,7 +3404,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="A1:E1"/>
@@ -3423,29 +3423,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" style="65" customWidth="1"/>
-    <col min="4" max="4" width="50.140625" customWidth="1"/>
-    <col min="5" max="5" width="24.140625" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" style="65" customWidth="1"/>
+    <col min="4" max="4" width="50.109375" customWidth="1"/>
+    <col min="5" max="5" width="24.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="124" t="s">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="118" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="124"/>
-      <c r="C1" s="124"/>
-      <c r="D1" s="124"/>
-      <c r="E1" s="124"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="14"/>
       <c r="B2" s="41"/>
       <c r="C2" s="68" t="s">
@@ -3454,7 +3454,7 @@
       <c r="D2" s="14"/>
       <c r="E2" s="14"/>
     </row>
-    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -3471,7 +3471,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="78">
         <v>1</v>
@@ -3482,7 +3482,7 @@
       <c r="D4" s="92"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="38" t="s">
         <v>4</v>
       </c>
@@ -3499,7 +3499,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="38"/>
       <c r="B6" s="39">
         <v>3</v>
@@ -3514,7 +3514,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="38"/>
       <c r="B7" s="39">
         <v>4</v>
@@ -3529,7 +3529,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="38" t="s">
         <v>8</v>
       </c>
@@ -3546,7 +3546,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="38"/>
       <c r="B9" s="39">
         <v>5</v>
@@ -3559,7 +3559,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="38"/>
       <c r="B10" s="39">
         <v>5</v>
@@ -3572,7 +3572,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="38"/>
       <c r="B11" s="39">
         <v>5</v>
@@ -3585,7 +3585,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="38"/>
       <c r="B12" s="39">
         <v>6</v>
@@ -3600,7 +3600,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="38"/>
       <c r="B13" s="39">
         <v>6</v>
@@ -3613,7 +3613,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="38"/>
       <c r="B14" s="39">
         <v>6</v>
@@ -3626,7 +3626,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="38"/>
       <c r="B15" s="39">
         <v>6</v>
@@ -3639,7 +3639,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="38"/>
       <c r="B16" s="39">
         <v>7</v>
@@ -3654,7 +3654,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="38"/>
       <c r="B17" s="39">
         <v>7</v>
@@ -3667,7 +3667,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="38"/>
       <c r="B18" s="39">
         <v>7</v>
@@ -3680,7 +3680,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="38"/>
       <c r="B19" s="39">
         <v>7</v>
@@ -3693,7 +3693,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="38"/>
       <c r="B20" s="39">
         <v>7</v>
@@ -3706,7 +3706,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="38"/>
       <c r="B21" s="39">
         <v>7</v>
@@ -3717,7 +3717,7 @@
       </c>
       <c r="E21" s="38"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="76"/>
       <c r="B22" s="77"/>
       <c r="C22" s="79">
@@ -3730,7 +3730,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="58" t="s">
         <v>99</v>
       </c>
@@ -3745,7 +3745,7 @@
       </c>
       <c r="E23" s="38"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="38" t="s">
         <v>12</v>
       </c>
@@ -3762,7 +3762,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="38"/>
       <c r="B25" s="39">
         <v>9</v>
@@ -3775,7 +3775,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="38"/>
       <c r="B26" s="39">
         <v>9</v>
@@ -3788,7 +3788,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="38"/>
       <c r="B27" s="39">
         <v>10</v>
@@ -3803,7 +3803,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="38" t="s">
         <v>13</v>
       </c>
@@ -3820,7 +3820,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="38"/>
       <c r="B29" s="39">
         <v>11</v>
@@ -3833,7 +3833,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="38"/>
       <c r="B30" s="39">
         <v>11</v>
@@ -3846,7 +3846,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="38"/>
       <c r="B31" s="40" t="s">
         <v>61</v>
@@ -3859,7 +3859,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="38" t="s">
         <v>14</v>
       </c>
@@ -3876,7 +3876,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="38"/>
       <c r="B33" s="39">
         <v>12</v>
@@ -3889,7 +3889,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="38"/>
       <c r="B34" s="39">
         <v>12</v>
@@ -3902,7 +3902,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="38"/>
       <c r="B35" s="39">
         <v>12</v>
@@ -3915,7 +3915,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="58" t="s">
         <v>55</v>
       </c>
@@ -3930,7 +3930,7 @@
       </c>
       <c r="E36" s="38"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="58" t="s">
         <v>78</v>
       </c>

</xml_diff>